<commit_message>
Added new tests and updated results excel
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arik Rinberg\Desktop\GitRepos\json-delta-crdt\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7359795D-54EF-4728-B31D-92543D2D9B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6542DDB-7DB9-4306-844D-F13B5BB404EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{07BF1D62-9602-4DD2-9B5A-FFE17FE3C19E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{07BF1D62-9602-4DD2-9B5A-FFE17FE3C19E}"/>
   </bookViews>
   <sheets>
     <sheet name="map-update" sheetId="1" r:id="rId1"/>
@@ -1731,94 +1731,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>493</c:v>
+                  <c:v>1260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>624</c:v>
+                  <c:v>1929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>789</c:v>
+                  <c:v>2612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>998</c:v>
+                  <c:v>3325</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1247</c:v>
+                  <c:v>4050</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1538</c:v>
+                  <c:v>4797</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1871</c:v>
+                  <c:v>5566</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2246</c:v>
+                  <c:v>6361</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2663</c:v>
+                  <c:v>7178</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3112</c:v>
+                  <c:v>8013</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3633</c:v>
+                  <c:v>8919</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4256</c:v>
+                  <c:v>9882</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4881</c:v>
+                  <c:v>10869</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5523</c:v>
+                  <c:v>11879</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6222</c:v>
+                  <c:v>12913</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6979</c:v>
+                  <c:v>14023</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7885</c:v>
+                  <c:v>15107</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8705</c:v>
+                  <c:v>16215</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9643</c:v>
+                  <c:v>17347</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10591</c:v>
+                  <c:v>18503</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11501</c:v>
+                  <c:v>19683</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12625</c:v>
+                  <c:v>20931</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13711</c:v>
+                  <c:v>22161</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14243</c:v>
+                  <c:v>23415</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16021</c:v>
+                  <c:v>24693</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17245</c:v>
+                  <c:v>25995</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18515</c:v>
+                  <c:v>27321</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>19803</c:v>
+                  <c:v>28671</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>21164</c:v>
+                  <c:v>30045</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>22546</c:v>
+                  <c:v>31448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4662,7 +4662,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4857,7 +4857,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1164062126642772"/>
+          <c:y val="3.172834389853315E-2"/>
+          <c:w val="0.7720676958390954"/>
+          <c:h val="0.71642348799967259"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -5246,7 +5256,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5295,7 +5305,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -5325,7 +5335,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -5354,7 +5364,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5405,7 +5415,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="2000">
+        <a:defRPr sz="2800">
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
@@ -19274,15 +19284,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19316,19 +19326,423 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.89451</cdr:y>
+      <cdr:x>0.01075</cdr:x>
+      <cdr:y>0.89256</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11587</cdr:x>
-      <cdr:y>1</cdr:y>
+      <cdr:x>0.12662</cdr:x>
+      <cdr:y>0.99805</cdr:y>
+    </cdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B661B78-65C6-41DE-A14A-38071737416B}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="142875" y="4361342"/>
+              <a:ext cx="1539608" cy="515458"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑢</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-IL" sz="2000"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B661B78-65C6-41DE-A14A-38071737416B}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="142875" y="4361342"/>
+              <a:ext cx="1539608" cy="515458"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:r>
+                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑝_𝑢</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-IL" sz="2000"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01595</cdr:x>
+      <cdr:y>0.75637</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11699</cdr:x>
+      <cdr:y>0.81665</cdr:y>
+    </cdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="3" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B393DAA4-8564-41C1-AC8C-1EBE2E2900DE}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="180975" y="3346450"/>
+              <a:ext cx="1146175" cy="266700"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:lvl1pPr marL="0" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑝</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑠</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-IL" sz="2000"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="3" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B393DAA4-8564-41C1-AC8C-1EBE2E2900DE}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="180975" y="3346450"/>
+              <a:ext cx="1146175" cy="266700"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:lvl1pPr marL="0" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" indent="0">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:r>
+                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑝_𝑠</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-IL" sz="2000"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.10579</cdr:x>
+      <cdr:y>0.08881</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.89319</cdr:x>
+      <cdr:y>0.08881</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0740FA43-239E-49F2-914F-FBFC9718E6DD}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1405671" y="433955"/>
+          <a:ext cx="10462480" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.85591</cdr:x>
+      <cdr:y>0.09706</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99642</cdr:x>
+      <cdr:y>0.18533</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
+        <cdr:cNvPr id="4" name="TextBox 3">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B661B78-65C6-41DE-A14A-38071737416B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFEEA9B8-3E1D-47A2-9DCD-2747239BCB60}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -19336,8 +19750,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="3957638"/>
-          <a:ext cx="1314450" cy="466725"/>
+          <a:off x="11372852" y="474253"/>
+          <a:ext cx="1866900" cy="431316"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -19348,29 +19762,79 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>p[Update]</a:t>
+            <a:rPr lang="en-US" sz="2800"/>
+            <a:t>Worst Case</a:t>
           </a:r>
-          <a:endParaRPr lang="en-IL" sz="2000"/>
+          <a:endParaRPr lang="en-IL" sz="2800"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.01595</cdr:x>
-      <cdr:y>0.75637</cdr:y>
+      <cdr:x>0.10859</cdr:x>
+      <cdr:y>0.5679</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11699</cdr:x>
-      <cdr:y>0.81665</cdr:y>
+      <cdr:x>0.89104</cdr:x>
+      <cdr:y>0.5679</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04AAE205-CA18-4E50-8470-695B12BDFAF1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1442905" y="2774950"/>
+          <a:ext cx="10396671" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.87885</cdr:x>
+      <cdr:y>0.46849</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.55676</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 1">
+        <cdr:cNvPr id="11" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B393DAA4-8564-41C1-AC8C-1EBE2E2900DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47707AF4-C6FB-4085-99B6-0B233B1D7314}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -19378,8 +19842,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="180975" y="3346450"/>
-          <a:ext cx="1146175" cy="266700"/>
+          <a:off x="11677650" y="2289175"/>
+          <a:ext cx="1609725" cy="431316"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -19454,63 +19918,13 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>p[Sync]</a:t>
+            <a:rPr lang="en-US" sz="2800"/>
+            <a:t>Best Case</a:t>
           </a:r>
-          <a:endParaRPr lang="en-IL" sz="2000"/>
+          <a:endParaRPr lang="en-IL" sz="2800"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.10243</cdr:x>
-      <cdr:y>0.03983</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.98573</cdr:x>
-      <cdr:y>0.04196</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="5" name="Straight Connector 4">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0740FA43-239E-49F2-914F-FBFC9718E6DD}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1162050" y="176214"/>
-          <a:ext cx="10020300" cy="9444"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
   </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
@@ -21145,8 +21559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D3E514-F1D7-4595-A703-2EBD73A0695A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21188,14 +21602,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>493</v>
+        <v>1260</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2">
         <f>B2/G2</f>
-        <v>493</v>
+        <v>1260</v>
       </c>
       <c r="I2">
         <f>C2/G2</f>
@@ -21211,14 +21625,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>624</v>
+        <v>1929</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="0">B3/G3</f>
-        <v>312</v>
+        <v>964.5</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="1">C3/G3</f>
@@ -21234,14 +21648,14 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>789</v>
+        <v>2612</v>
       </c>
       <c r="G4" s="1">
         <v>4</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>197.25</v>
+        <v>653</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
@@ -21257,14 +21671,14 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>998</v>
+        <v>3325</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>124.75</v>
+        <v>415.625</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
@@ -21280,14 +21694,14 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1247</v>
+        <v>4050</v>
       </c>
       <c r="G6" s="1">
         <v>16</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>77.9375</v>
+        <v>253.125</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -21303,14 +21717,14 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1538</v>
+        <v>4797</v>
       </c>
       <c r="G7" s="1">
         <v>32</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>48.0625</v>
+        <v>149.90625</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
@@ -21326,14 +21740,14 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1871</v>
+        <v>5566</v>
       </c>
       <c r="G8" s="1">
         <v>64</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>29.234375</v>
+        <v>86.96875</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
@@ -21349,14 +21763,14 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2246</v>
+        <v>6361</v>
       </c>
       <c r="G9" s="1">
         <v>128</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>17.546875</v>
+        <v>49.6953125</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
@@ -21372,14 +21786,14 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2663</v>
+        <v>7178</v>
       </c>
       <c r="G10" s="1">
         <v>256</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>10.40234375</v>
+        <v>28.0390625</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
@@ -21395,14 +21809,14 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3112</v>
+        <v>8013</v>
       </c>
       <c r="G11" s="1">
         <v>512</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>6.078125</v>
+        <v>15.650390625</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
@@ -21418,7 +21832,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3633</v>
+        <v>8919</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -21427,7 +21841,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4256</v>
+        <v>9882</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -21436,7 +21850,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4881</v>
+        <v>10869</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -21445,7 +21859,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5523</v>
+        <v>11879</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -21454,7 +21868,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>6222</v>
+        <v>12913</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -21463,7 +21877,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>6979</v>
+        <v>14023</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -21472,7 +21886,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>7885</v>
+        <v>15107</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -21481,7 +21895,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>8705</v>
+        <v>16215</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -21490,7 +21904,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>9643</v>
+        <v>17347</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -21499,7 +21913,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>10591</v>
+        <v>18503</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -21508,7 +21922,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>11501</v>
+        <v>19683</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -21516,7 +21930,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>12625</v>
+        <v>20931</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -21524,7 +21938,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>13711</v>
+        <v>22161</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -21532,7 +21946,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>14243</v>
+        <v>23415</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -21540,7 +21954,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>16021</v>
+        <v>24693</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -21548,7 +21962,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>17245</v>
+        <v>25995</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -21556,7 +21970,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>18515</v>
+        <v>27321</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -21564,7 +21978,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>19803</v>
+        <v>28671</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -21572,7 +21986,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>21164</v>
+        <v>30045</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -21580,7 +21994,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>22546</v>
+        <v>31448</v>
       </c>
     </row>
   </sheetData>
@@ -21594,7 +22008,7 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26675,8 +27089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27F1933-2C52-4CFD-9A50-6792B5A0F67D}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33508,7 +33922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A78244-549C-4DC9-8ABB-39AC803B5CE3}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated test and results
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arik Rinberg\Desktop\GitRepos\json-delta-crdt\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6542DDB-7DB9-4306-844D-F13B5BB404EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E74732-9D8A-46C8-B3A3-25B0236C33E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{07BF1D62-9602-4DD2-9B5A-FFE17FE3C19E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{07BF1D62-9602-4DD2-9B5A-FFE17FE3C19E}"/>
   </bookViews>
   <sheets>
     <sheet name="map-update" sheetId="1" r:id="rId1"/>
@@ -1856,7 +1856,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1885,7 +1885,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -1920,7 +1920,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1968,7 +1968,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -1997,7 +1997,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -2026,7 +2026,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2076,7 +2076,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="2000">
+        <a:defRPr sz="2800">
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
@@ -5256,7 +5256,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5305,7 +5305,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -5335,7 +5335,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -5364,7 +5364,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5415,7 +5415,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="2800">
+        <a:defRPr sz="3200">
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
@@ -7086,58 +7086,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>493</c:v>
+                  <c:v>483</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>507</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>514</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>514</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>515</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>516</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>516</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>516</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>516</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>516</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>533</c:v>
+                  <c:v>522</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>533</c:v>
+                  <c:v>522</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>533</c:v>
+                  <c:v>522</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>534</c:v>
+                  <c:v>523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7422,7 +7422,7 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>46</c:v>
@@ -7434,7 +7434,7 @@
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>51</c:v>
@@ -7452,7 +7452,7 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>57</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>58</c:v>
@@ -19283,16 +19283,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19333,8 +19333,8 @@
       <cdr:x>0.12662</cdr:x>
       <cdr:y>0.99805</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1">
@@ -19369,14 +19369,14 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑝</m:t>
@@ -19384,7 +19384,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑢</m:t>
@@ -19394,12 +19394,12 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-IL" sz="2000"/>
+              <a:endParaRPr lang="en-IL" sz="2800"/>
             </a:p>
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1">
@@ -19424,13 +19424,14 @@
             <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
             <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
             <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:pPr/>
               <a:r>
-                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                <a:rPr lang="en-US" sz="2800" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑝_𝑢</a:t>
               </a:r>
-              <a:endParaRPr lang="en-IL" sz="2000"/>
+              <a:endParaRPr lang="en-IL" sz="2800"/>
             </a:p>
           </cdr:txBody>
         </cdr:sp>
@@ -19446,8 +19447,8 @@
       <cdr:x>0.11699</cdr:x>
       <cdr:y>0.81665</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="3" name="TextBox 1">
@@ -19546,14 +19547,14 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑝</m:t>
@@ -19561,7 +19562,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="2000" b="0" i="1">
+                          <a:rPr lang="en-US" sz="2800" b="0" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                           <m:t>𝑠</m:t>
@@ -19571,12 +19572,12 @@
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-IL" sz="2000"/>
+              <a:endParaRPr lang="en-IL" sz="2800"/>
             </a:p>
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="3" name="TextBox 1">
@@ -19665,13 +19666,14 @@
               </a:lvl9pPr>
             </a:lstStyle>
             <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:pPr/>
               <a:r>
-                <a:rPr lang="en-US" sz="2000" b="0" i="0">
+                <a:rPr lang="en-US" sz="2800" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑝_𝑠</a:t>
               </a:r>
-              <a:endParaRPr lang="en-IL" sz="2000"/>
+              <a:endParaRPr lang="en-IL" sz="2800"/>
             </a:p>
           </cdr:txBody>
         </cdr:sp>
@@ -20573,7 +20575,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21559,8 +21561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D3E514-F1D7-4595-A703-2EBD73A0695A}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24545,7 +24547,7 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27089,8 +27091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27F1933-2C52-4CFD-9A50-6792B5A0F67D}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31210,7 +31212,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31790,8 +31792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5A9AA3-DEAB-4253-9BB3-43727FED9685}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31833,7 +31835,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C2">
         <v>784</v>
@@ -31862,7 +31864,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C3">
         <v>1023</v>
@@ -31891,7 +31893,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C4">
         <v>1501</v>
@@ -31920,7 +31922,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C5">
         <v>2457</v>
@@ -31949,7 +31951,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="C6">
         <v>4383</v>
@@ -31978,7 +31980,7 @@
         <v>32</v>
       </c>
       <c r="B7">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="C7">
         <v>8239</v>
@@ -31991,7 +31993,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1.028397565922921</v>
+        <v>1.0269151138716357</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -32007,20 +32009,20 @@
         <v>64</v>
       </c>
       <c r="B8">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C8">
         <v>15951</v>
       </c>
       <c r="D8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1">
         <v>64</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1.0425963488843812</v>
+        <v>1.0414078674948239</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -32028,7 +32030,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>1.075</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -32036,7 +32038,7 @@
         <v>128</v>
       </c>
       <c r="B9">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C9">
         <v>31433</v>
@@ -32049,7 +32051,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1.0425963488843812</v>
+        <v>1.0414078674948239</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -32065,7 +32067,7 @@
         <v>256</v>
       </c>
       <c r="B10">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="C10">
         <v>62537</v>
@@ -32078,7 +32080,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>1.0446247464503042</v>
+        <v>1.0434782608695652</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
@@ -32094,7 +32096,7 @@
         <v>512</v>
       </c>
       <c r="B11">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="C11">
         <v>124745</v>
@@ -32107,7 +32109,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1.0466531440162272</v>
+        <v>1.0455486542443064</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
@@ -32123,20 +32125,20 @@
         <v>1024</v>
       </c>
       <c r="B12">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="C12">
         <v>249211</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1">
         <v>1024</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1.0466531440162272</v>
+        <v>1.0455486542443064</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
@@ -32144,7 +32146,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>1.2749999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -32152,7 +32154,7 @@
         <v>2048</v>
       </c>
       <c r="B13">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="C13">
         <v>500091</v>
@@ -32165,7 +32167,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>1.0466531440162272</v>
+        <v>1.0455486542443064</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
@@ -32181,7 +32183,7 @@
         <v>4096</v>
       </c>
       <c r="B14">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="C14">
         <v>1001851</v>
@@ -32194,7 +32196,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1.0466531440162272</v>
+        <v>1.0455486542443064</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
@@ -32210,7 +32212,7 @@
         <v>8192</v>
       </c>
       <c r="B15">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="C15">
         <v>2005371</v>
@@ -32223,7 +32225,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1.0466531440162272</v>
+        <v>1.0455486542443064</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
@@ -32239,7 +32241,7 @@
         <v>16384</v>
       </c>
       <c r="B16">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="C16">
         <v>4025181</v>
@@ -32252,7 +32254,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>1.0811359026369169</v>
+        <v>1.0807453416149069</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
@@ -32268,7 +32270,7 @@
         <v>32768</v>
       </c>
       <c r="B17">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="C17">
         <v>8072029</v>
@@ -32281,7 +32283,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>1.0811359026369169</v>
+        <v>1.0807453416149069</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
@@ -32297,20 +32299,20 @@
         <v>65536</v>
       </c>
       <c r="B18">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="C18">
         <v>16165725</v>
       </c>
       <c r="D18">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18" s="1">
         <v>65536</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>1.0811359026369169</v>
+        <v>1.0807453416149069</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
@@ -32318,7 +32320,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>1.425</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -32326,7 +32328,7 @@
         <v>131072</v>
       </c>
       <c r="B19">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="C19">
         <v>32415263</v>
@@ -32339,7 +32341,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>1.0831643002028397</v>
+        <v>1.0828157349896481</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
@@ -32843,7 +32845,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33383,7 +33385,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33923,7 +33925,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>